<commit_message>
Final Change in framework for ION
</commit_message>
<xml_diff>
--- a/TestSuite.xlsx
+++ b/TestSuite.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="75">
   <si>
     <t>ExecutionStatus</t>
   </si>
@@ -250,9 +250,6 @@
   </si>
   <si>
     <t>Android_6.0</t>
-  </si>
-  <si>
-    <t>Android_7.1</t>
   </si>
 </sst>
 </file>
@@ -870,7 +867,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -944,19 +941,19 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>66</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>36</v>
@@ -973,7 +970,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>71</v>
@@ -1001,7 +998,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="7">
+  <dataValidations count="8">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Should n`t be empty" promptTitle="Select OS" sqref="B5:C14">
       <formula1>OS</formula1>
     </dataValidation>
@@ -1017,11 +1014,14 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
       <formula1>"Web,Android,iOS"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2:B4">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
       <formula1>"webApp,nativeApp,sanityTesting"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
       <formula1>"Windows_Chrome,Windows_Firefox,Windows_Safari,Android_6.0,Android_7.1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"webApp,NativeApp,sanityTesting"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Completed Add user scenarios with all queries access cases
</commit_message>
<xml_diff>
--- a/TestSuite.xlsx
+++ b/TestSuite.xlsx
@@ -228,28 +228,28 @@
     <t>None</t>
   </si>
   <si>
+    <t>Exec</t>
+  </si>
+  <si>
+    <t>Web</t>
+  </si>
+  <si>
+    <t>AppType</t>
+  </si>
+  <si>
+    <t>webApp</t>
+  </si>
+  <si>
+    <t>Sanity</t>
+  </si>
+  <si>
+    <t>Android_6.1</t>
+  </si>
+  <si>
     <t>Windows_Chrome</t>
   </si>
   <si>
-    <t>Exec</t>
-  </si>
-  <si>
-    <t>Web</t>
-  </si>
-  <si>
-    <t>AppType</t>
-  </si>
-  <si>
-    <t>webApp</t>
-  </si>
-  <si>
-    <t>Sanity</t>
-  </si>
-  <si>
-    <t>nativeApp</t>
-  </si>
-  <si>
-    <t>Android_6.0</t>
+    <t>ZY32288VFB</t>
   </si>
 </sst>
 </file>
@@ -867,7 +867,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -883,10 +883,10 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -907,24 +907,24 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F2" s="12" t="s">
         <v>36</v>
@@ -941,22 +941,22 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>28</v>
@@ -973,25 +973,25 @@
         <v>28</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>66</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>28</v>
@@ -1008,20 +1008,20 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Should n`t be empty" sqref="A2:A4">
       <formula1>"Run,No"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
-      <formula1>"None,emulator-5554,emulator-5556"</formula1>
-    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C2:C4">
       <formula1>"Web,Android,iOS"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B3:B4">
       <formula1>"webApp,nativeApp,sanityTesting"</formula1>
     </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>"webApp,nativeApp,sanityTesting"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D4">
-      <formula1>"Windows_Chrome,Windows_Firefox,Windows_Safari,Android_6.0,Android_7.1"</formula1>
+      <formula1>"Windows_Chrome,Windows_Firefox,Windows_Safari,Android_6.0,Android_7.1,Android_5.0"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B2">
-      <formula1>"webApp,NativeApp,sanityTesting"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:E4">
+      <formula1>"None,emulator-5554,emulator-5556,b1a1589f,ZY32288VFB"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>